<commit_message>
add pearson correlation as score
</commit_message>
<xml_diff>
--- a/MHCI_BP_predictor/ExistStart_roc_auc.xlsx
+++ b/MHCI_BP_predictor/ExistStart_roc_auc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mxdwa\Documents\code\MHC-peptide_prediction\MHCI_BP_predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{995F9475-ABA9-4020-BAB7-A1714E157D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2EC768C2-9D94-4DC0-B7F0-D19485A19603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>1-round</t>
   </si>
@@ -80,6 +80,14 @@
   </si>
   <si>
     <t>20-round</t>
+  </si>
+  <si>
+    <t>H-2-Kd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>H-2-Kb</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1040,136 +1048,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A3">
         <v>0.73792600024919897</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>0.75479050696208905</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>0.76488854176379295</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>0.77604624533843103</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E3" s="1">
         <v>0.77348164238174699</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>0.76974833373674001</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>0.76673036733330602</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>0.76918097398718099</v>
       </c>
-      <c r="I2">
+      <c r="I3">
         <v>0.77155711452515996</v>
       </c>
-      <c r="J2">
+      <c r="J3">
         <v>0.76619308222937299</v>
       </c>
-      <c r="K2">
+      <c r="K3">
         <v>0.765110921058062</v>
       </c>
-      <c r="L2">
+      <c r="L3">
         <v>0.76774118837094596</v>
       </c>
-      <c r="M2">
+      <c r="M3">
         <v>0.73706255366429696</v>
       </c>
-      <c r="N2">
+      <c r="N3">
         <v>0.75815880538967395</v>
       </c>
-      <c r="O2">
+      <c r="O3">
         <v>0.753390936154271</v>
       </c>
-      <c r="P2">
+      <c r="P3">
         <v>0.74769444764798598</v>
       </c>
-      <c r="Q2">
+      <c r="Q3">
         <v>0.77179031475999205</v>
       </c>
-      <c r="R2">
+      <c r="R3">
         <v>0.75932387725329897</v>
       </c>
-      <c r="S2">
+      <c r="S3">
         <v>0.75111215332830406</v>
       </c>
-      <c r="T2">
+      <c r="T3">
         <v>0.74381081220812295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>0.80439628137903896</v>
+      </c>
+      <c r="B6">
+        <v>0.80698228033022501</v>
+      </c>
+      <c r="C6">
+        <v>0.80998924469505496</v>
+      </c>
+      <c r="D6">
+        <v>0.80771853238971703</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.80949232742986799</v>
+      </c>
+      <c r="F6">
+        <v>0.80749432802905796</v>
+      </c>
+      <c r="G6">
+        <v>0.81200344057695595</v>
+      </c>
+      <c r="H6">
+        <v>0.80146176962877402</v>
+      </c>
+      <c r="I6">
+        <v>0.80798236409357804</v>
+      </c>
+      <c r="J6">
+        <v>0.80706128250817399</v>
+      </c>
+      <c r="K6">
+        <v>0.81322693708600402</v>
+      </c>
+      <c r="L6">
+        <v>0.80572021388874904</v>
+      </c>
+      <c r="M6">
+        <v>0.81479722236245999</v>
+      </c>
+      <c r="N6">
+        <v>0.816846977161093</v>
+      </c>
+      <c r="O6">
+        <v>0.81164607310565295</v>
+      </c>
+      <c r="P6">
+        <v>0.80948464482669602</v>
+      </c>
+      <c r="Q6">
+        <v>0.80946574356911105</v>
+      </c>
+      <c r="R6">
+        <v>0.81247017338392502</v>
+      </c>
+      <c r="S6">
+        <v>0.809821259631885</v>
+      </c>
+      <c r="T6">
+        <v>0.81240935974595296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>